<commit_message>
continued to work on elemental affinities, tags and materials. had to delete the step dice spreadsheet because of a vba macro bug.
</commit_message>
<xml_diff>
--- a/Materials and Crafting.xlsx
+++ b/Materials and Crafting.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metals" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="482">
   <si>
     <t xml:space="preserve">METAL</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- -</t>
   </si>
   <si>
     <t xml:space="preserve">erebian resonance 1
@@ -226,9 +229,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mercury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- -</t>
   </si>
   <si>
     <t xml:space="preserve">aquan resonance 1
@@ -362,7 +362,6 @@
   </si>
   <si>
     <t xml:space="preserve">luthian affinity 6
-radiant affinity 4
 arcing 3
 flaming 3
 siege metal
@@ -382,8 +381,10 @@
     <t xml:space="preserve">Nulgrulite</t>
   </si>
   <si>
+    <t xml:space="preserve">- - - - -</t>
+  </si>
+  <si>
     <t xml:space="preserve">erebian affinity 6
-necrotic affinity 4
 vampiric 3
 antimagic 9
 weave eating
@@ -391,7 +392,7 @@
 crystalline</t>
   </si>
   <si>
-    <t xml:space="preserve">This crystal is uterrly black, like a void in space. All things that contact it are disintegrated, vanishing as if they were never there.</t>
+    <t xml:space="preserve">This crystal is utterly black, like a void in space. All things that contact it are disintegrated, vanishing as if they were never there.</t>
   </si>
   <si>
     <t xml:space="preserve">See 'Arctanite' glass</t>
@@ -425,7 +426,7 @@
     <t xml:space="preserve">Necrodermis</t>
   </si>
   <si>
-    <t xml:space="preserve">- - - - -</t>
+    <t xml:space="preserve">- - - -</t>
   </si>
   <si>
     <t xml:space="preserve">necrotic affinity 4
@@ -451,10 +452,17 @@
     <t xml:space="preserve">See 'Plagueshell' leather</t>
   </si>
   <si>
+    <t xml:space="preserve">See 'Dragonscale' leather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See 'Nullscale' leather</t>
+  </si>
+  <si>
     <t xml:space="preserve">Celesteel</t>
   </si>
   <si>
-    <t xml:space="preserve">elysian affinity 2
+    <t xml:space="preserve">luthian affinity 1
+elysian affinity 2
 healing affinity 2
 weightless</t>
   </si>
@@ -468,7 +476,8 @@
     <t xml:space="preserve">Celesturum</t>
   </si>
   <si>
-    <t xml:space="preserve">elysian affinity 4
+    <t xml:space="preserve">luthian affinity 2
+elysian affinity 4
 healing affinity 4
 weightless</t>
   </si>
@@ -480,7 +489,8 @@
     <t xml:space="preserve">Stygian Iron</t>
   </si>
   <si>
-    <t xml:space="preserve">hadean affinity 2
+    <t xml:space="preserve">erebian affinity 1
+hadean affinity 2
 keen 2
 brittle</t>
   </si>
@@ -494,7 +504,8 @@
     <t xml:space="preserve">Stygian Steel</t>
   </si>
   <si>
-    <t xml:space="preserve">hadean affinity 4
+    <t xml:space="preserve">erebian affinity 2
+hadean affinity 4
 keen 4
 vampiric</t>
   </si>
@@ -598,90 +609,100 @@
     <t xml:space="preserve">primal resonance 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Harvest from the corpse of a beast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 – 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">A tanned hide from a particular non-magical beast.</t>
   </si>
   <si>
     <t xml:space="preserve">Monstrosity</t>
   </si>
   <si>
-    <t xml:space="preserve">CR / 10</t>
+    <t xml:space="preserve">CR / 5</t>
   </si>
   <si>
     <t xml:space="preserve">~</t>
   </si>
   <si>
-    <t xml:space="preserve">CR / 3</t>
+    <t xml:space="preserve">Harvest from the corpse of a monstrosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 – 12</t>
   </si>
   <si>
     <t xml:space="preserve">A tanned hide from a creature borne from or suffused with magic.</t>
   </si>
   <si>
+    <t xml:space="preserve">Rotflesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">necrotic affinity 1 – 3
+putrefied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from a destroyed corporeal undead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 – 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fetid leather, tanned from the rotting skin of an undead corpse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angelflesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elysian affinity 1 – 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a celestial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hellskin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hadean affinity 1 – 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a fiend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warp Flesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psychic affinity 1 – 3
+eldritch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of an aberration</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stoneskin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- - - -</t>
   </si>
   <si>
     <t xml:space="preserve">terran affinity 1
 physical affinity 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Harvest from a gargoyle or tomb guardian</t>
+    <t xml:space="preserve">Harvest from the corpse of a gargoyle or tomb guardian</t>
   </si>
   <si>
     <t xml:space="preserve">A strange leather that appears as if it were petrified, encased with a thin layer of stone. Strange patterns swirl form cracks through its surface.</t>
   </si>
   <si>
-    <t xml:space="preserve">Dragonscale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">colour affinity (CR / 4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvest from the corpse of a metallic or chromatic dragon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The scaled leather from an extinct dragon. It flows with residual magical energy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necrosil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erebian affinity (CR / 4)
-shadowwrit
-dusk delay
-sharp 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvest from a sentient shadow creature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A sharp, stringy leather hued with the deep black of shadows, which flit and dance across its surface.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plagueshell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erebian affinity 3
-poison affinity 3
-toxic 4
-metallic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvest from a plaguebringer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A strong but flexible dark chitin plating that emits a noxious smog. It is tainted by the energies of the shadowfell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warp Flesh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">psychic affinity (CR / 4)
-eldritch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvest from an abberation</t>
+    <t xml:space="preserve">Wyrmscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">superior 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a lesser dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The leathery scale of a lesser dragon such as a wyvern, pseudodragon or drake.</t>
   </si>
   <si>
     <t xml:space="preserve">Chlorophyte</t>
@@ -746,6 +767,65 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Ectoplasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from a destroyed ethereal undead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A glassy leather tanned from the phantasmal skin of a ghost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragonscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colour affinity 1 – 3
+superior 1
+metallic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a true dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 / 10 / 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scaled leather from an extinct true dragon. It flows with residual magical energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necrosil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erebian affinity 1 – 3
+shadowwrit
+dusk delay
+sharp 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a creature with shadow stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 – 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A sharp, stringy leather hued with the deep black of shadows, which flit and dance across its surface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plagueshell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erebian affinity 3
+poison affinity 3
+toxic 4
+metallic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a plaguebringer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A strong but flexible dark chitin plating that emits a noxious smog. It is tainted by the energies of the shadowfell.</t>
+  </si>
+  <si>
     <t xml:space="preserve">See 'Orichalcum' metal</t>
   </si>
   <si>
@@ -753,10 +833,11 @@
   </si>
   <si>
     <t xml:space="preserve">nyxian affinity 3
+healing affinity 3
 siege metal</t>
   </si>
   <si>
-    <t xml:space="preserve">Harvest from an astral dragon</t>
+    <t xml:space="preserve">Harvest from the corpse of an astral dragon</t>
   </si>
   <si>
     <t xml:space="preserve">15,000 gp</t>
@@ -772,7 +853,22 @@
 arboreal</t>
   </si>
   <si>
-    <t xml:space="preserve">Harvest from an overseer</t>
+    <t xml:space="preserve">Harvest from the corpse of an overseer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nullscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erebian affinity 2 / 3 / 4
+antimagic 5 / 7 / 9
+superior 1
+metallic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvest from the corpse of a void dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 / 16 / 20</t>
   </si>
   <si>
     <t xml:space="preserve">WOOD</t>
@@ -945,7 +1041,6 @@
   <si>
     <t xml:space="preserve">resonant 5
 animus affinity 1
-nyxian affinity 1
 brittle</t>
   </si>
   <si>
@@ -1592,8 +1687,7 @@
   </si>
   <si>
     <t xml:space="preserve">resonant 3
-animus affinity 2
-nyxian affinity 2</t>
+animus affinity 2</t>
   </si>
   <si>
     <t xml:space="preserve">Crystallise Soulshards</t>
@@ -1674,6 +1768,12 @@
   <si>
     <t xml:space="preserve">toxic 4
 acid affinity 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endoplasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animus affinity 1</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1866,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1807,6 +1907,13 @@
       <right/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1987,8 +2094,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1999,16 +2114,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2021,10 +2136,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2063,10 +2174,6 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2075,7 +2182,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -13838,15 +13945,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
@@ -13903,7 +14010,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>12</v>
@@ -13929,7 +14036,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>16</v>
@@ -13958,7 +14065,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>16</v>
@@ -13987,7 +14094,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>26</v>
@@ -14013,7 +14120,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>30</v>
@@ -14042,7 +14149,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>35</v>
@@ -14068,7 +14175,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>40</v>
@@ -14092,7 +14199,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>46</v>
@@ -14142,7 +14249,7 @@
         <v>55</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>56</v>
@@ -14159,27 +14266,27 @@
         <v>49</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>49</v>
@@ -14189,10 +14296,10 @@
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="27" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H13" s="26" t="s">
         <v>65</v>
@@ -14215,7 +14322,7 @@
         <v>68</v>
       </c>
       <c r="F14" s="17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>69</v>
@@ -14239,7 +14346,7 @@
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="17" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>72</v>
@@ -14263,7 +14370,7 @@
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="17" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>76</v>
@@ -14299,7 +14406,7 @@
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="3" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>81</v>
@@ -14322,7 +14429,7 @@
         <v>85</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>86</v>
@@ -14345,7 +14452,7 @@
         <v>89</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>90</v>
@@ -14368,7 +14475,7 @@
         <v>93</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>94</v>
@@ -14377,7 +14484,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="29" t="s">
         <v>96</v>
       </c>
@@ -14394,7 +14501,7 @@
         <v>98</v>
       </c>
       <c r="F22" s="17" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G22" s="32" t="s">
         <v>9</v>
@@ -14403,33 +14510,33 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
         <v>100</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="19" t="n">
-        <v>0</v>
+      <c r="C23" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="3" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G23" s="32" t="s">
         <v>9</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
@@ -14441,33 +14548,33 @@
     </row>
     <row r="25" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>84</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
@@ -14479,7 +14586,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -14491,33 +14598,33 @@
     </row>
     <row r="28" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F28" s="3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
@@ -14527,183 +14634,161 @@
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
     </row>
-    <row r="30" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="14" t="n">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+    </row>
+    <row r="32" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="17" t="n">
-        <v>6</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>121</v>
+      <c r="D32" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="B31" s="14" t="s">
+    <row r="33" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G32" s="4" t="s">
+      <c r="E33" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="F33" s="3" t="n">
         <v>10</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>8</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B34" s="14" t="n">
-        <v>0</v>
+        <v>128</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F34" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F35" s="3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G35" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="B37" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F36" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="F37" s="3" t="n">
         <v>10</v>
@@ -14712,15 +14797,63 @@
         <v>9</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
   </mergeCells>
-  <conditionalFormatting sqref="C14 C16 B28:C28 B30:C36 C18:C20 B22:C22 B25:C25 H8:I9 I10 H11:I16 I17 H28:I28 I26:I27 H30:I1048576 I29 H18:I23 H25:I25 I24">
+  <conditionalFormatting sqref="C14 C16 B28:C28 B32:C38 C18:C20 B22:C22 B25:C25 H8:I9 I10 H11:I16 I17 H28:I28 I26:I27 H32:I1048576 I29:I31 H18:I23 H25:I25 I24">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -14752,7 +14885,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C39">
     <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -14816,7 +14949,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+  <conditionalFormatting sqref="B39">
     <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15215,20 +15348,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="29.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="54.86"/>
@@ -15236,7 +15369,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -15260,9 +15393,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0</v>
@@ -15271,280 +15404,418 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>150</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="E3" s="36" t="s">
+        <v>157</v>
+      </c>
       <c r="F3" s="28" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>154</v>
+    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="37" t="s">
+        <v>160</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>156</v>
+      <c r="D4" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>2</v>
+        <v>162</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="15" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>49</v>
+    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="14" t="n">
+        <v>0</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>160</v>
+      <c r="D5" s="20" t="s">
+        <v>166</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>6</v>
+        <v>167</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="G5" s="11"/>
-      <c r="H5" s="15" t="s">
-        <v>162</v>
-      </c>
+      <c r="H5" s="15"/>
     </row>
-    <row r="6" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>6</v>
-      </c>
       <c r="G6" s="11"/>
-      <c r="H6" s="15" t="s">
-        <v>166</v>
-      </c>
+      <c r="H6" s="15"/>
     </row>
-    <row r="7" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="14" t="s">
+    <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="F7" s="17" t="n">
+      <c r="D7" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="15" t="s">
-        <v>170</v>
+      <c r="G8" s="11"/>
+      <c r="H8" s="15" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
-        <v>174</v>
+    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="37" t="s">
+        <v>178</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>5</v>
+      <c r="D10" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="14" t="s">
+    <row r="11" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H10" s="22"/>
+      <c r="D11" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" s="22"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+    <row r="12" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="15" t="s">
+        <v>190</v>
+      </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="B12" s="14" t="s">
+    <row r="13" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F12" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>184</v>
+      <c r="D17" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>209</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="B13" s="14" t="s">
+    <row r="18" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="F13" s="17" t="n">
-        <v>8</v>
+      <c r="D18" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="17" t="n">
+        <v>17</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="11"/>
-      <c r="H14" s="15"/>
+    <row r="19" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G22" s="32"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="32"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="32"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="32"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G31" s="32"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="32"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="32"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="32"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G35" s="32"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="32"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G37" s="32"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="32"/>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A16:H16"/>
   </mergeCells>
-  <conditionalFormatting sqref="C6 B2:C4">
+  <conditionalFormatting sqref="C14 B8:C9 B2:C3 B5:C6 B12">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15576,7 +15847,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="B14">
     <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15608,7 +15879,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
+  <conditionalFormatting sqref="C7">
     <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15640,7 +15911,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
+  <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15672,7 +15943,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C10">
     <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15704,7 +15975,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
+  <conditionalFormatting sqref="B10">
     <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15736,7 +16007,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+  <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" priority="62" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15768,7 +16039,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
+  <conditionalFormatting sqref="B11">
     <cfRule type="cellIs" priority="72" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15800,7 +16071,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
+  <conditionalFormatting sqref="B15:C15">
     <cfRule type="cellIs" priority="82" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15832,7 +16103,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
+  <conditionalFormatting sqref="H20:H1048576 H7 H10">
     <cfRule type="cellIs" priority="92" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15864,7 +16135,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C7">
+  <conditionalFormatting sqref="H3:H6 H12:H14 H8:H9">
     <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15896,7 +16167,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H9 H14:H1048576">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" priority="112" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15928,7 +16199,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H6">
+  <conditionalFormatting sqref="B17:C17">
     <cfRule type="cellIs" priority="122" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15960,7 +16231,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H17">
     <cfRule type="cellIs" priority="132" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -15992,7 +16263,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:C12">
+  <conditionalFormatting sqref="G3">
     <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -16024,7 +16295,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+  <conditionalFormatting sqref="H18:H19">
     <cfRule type="cellIs" priority="152" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -16056,7 +16327,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
+  <conditionalFormatting sqref="B18:B19">
     <cfRule type="cellIs" priority="162" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -16088,7 +16359,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="C18:C19">
     <cfRule type="cellIs" priority="172" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -16120,7 +16391,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="C12:C13">
     <cfRule type="cellIs" priority="182" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -16152,7 +16423,7 @@
       <formula>"- - - - -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="B13 B4:C4">
     <cfRule type="cellIs" priority="192" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340">
       <formula>"+ + + + +"</formula>
     </cfRule>
@@ -16207,7 +16478,7 @@
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
@@ -16219,7 +16490,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -16245,7 +16516,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0</v>
@@ -16265,7 +16536,7 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>9</v>
@@ -16274,20 +16545,20 @@
         <v>10</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="H3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -16296,20 +16567,20 @@
         <v>0</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="H4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="27" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>9</v>
@@ -16317,33 +16588,33 @@
       <c r="C5" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" s="41"/>
+      <c r="D5" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="E5" s="36"/>
       <c r="F5" s="27" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
-        <v>198</v>
+      <c r="A6" s="37" t="s">
+        <v>227</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="F6" s="17" t="n">
         <v>3</v>
@@ -16352,8 +16623,8 @@
       <c r="H6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
-        <v>201</v>
+      <c r="A7" s="37" t="s">
+        <v>230</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>19</v>
@@ -16362,10 +16633,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="F7" s="17" t="n">
         <v>4</v>
@@ -16374,8 +16645,8 @@
       <c r="H7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
-        <v>204</v>
+      <c r="A8" s="37" t="s">
+        <v>233</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>10</v>
@@ -16384,18 +16655,18 @@
         <v>0</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="F8" s="17" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
-        <v>207</v>
+      <c r="A9" s="37" t="s">
+        <v>236</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>38</v>
@@ -16404,18 +16675,18 @@
         <v>38</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="F9" s="17" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
-        <v>210</v>
+      <c r="A10" s="39" t="s">
+        <v>239</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>10</v>
@@ -16424,10 +16695,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>212</v>
+        <v>240</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>241</v>
       </c>
       <c r="F10" s="17" t="n">
         <v>4</v>
@@ -16436,7 +16707,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
@@ -16448,7 +16719,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
@@ -16982,13 +17253,13 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
@@ -17001,7 +17272,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -17027,7 +17298,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0</v>
@@ -17036,7 +17307,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="3" t="n">
@@ -17049,7 +17320,7 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="B3" s="14" t="n">
         <v>0</v>
@@ -17058,19 +17329,19 @@
         <v>38</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -17079,19 +17350,19 @@
         <v>10</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="H4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="27" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>10</v>
@@ -17099,21 +17370,21 @@
       <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>223</v>
+      <c r="D5" s="36" t="s">
+        <v>252</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27" t="n">
         <v>3</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>224</v>
+        <v>253</v>
       </c>
       <c r="H5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
-        <v>225</v>
+      <c r="A6" s="37" t="s">
+        <v>254</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>10</v>
@@ -17122,10 +17393,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="F6" s="17" t="n">
         <v>5</v>
@@ -17134,8 +17405,8 @@
       <c r="H6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
-        <v>228</v>
+      <c r="A7" s="43" t="s">
+        <v>257</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>9</v>
@@ -17144,10 +17415,10 @@
         <v>49</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
       <c r="F7" s="17" t="n">
         <v>6</v>
@@ -17156,8 +17427,8 @@
       <c r="H7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
-        <v>231</v>
+      <c r="A8" s="43" t="s">
+        <v>260</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>38</v>
@@ -17166,7 +17437,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="17"/>
@@ -17174,8 +17445,8 @@
       <c r="H8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
-        <v>233</v>
+      <c r="A9" s="43" t="s">
+        <v>262</v>
       </c>
       <c r="B9" s="19" t="n">
         <v>0</v>
@@ -17184,7 +17455,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>234</v>
+        <v>263</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -17193,7 +17464,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>235</v>
+        <v>264</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -17203,9 +17474,9 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
     </row>
-    <row r="11" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
-        <v>236</v>
+    <row r="11" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="37" t="s">
+        <v>265</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>43</v>
@@ -17214,18 +17485,18 @@
         <v>84</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>237</v>
+        <v>266</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
@@ -17520,7 +17791,7 @@
       <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
@@ -17532,7 +17803,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>241</v>
+        <v>270</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -17558,7 +17829,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>242</v>
+        <v>271</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0</v>
@@ -17566,8 +17837,8 @@
       <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="11" t="n">
         <v>0</v>
       </c>
@@ -17577,8 +17848,8 @@
       <c r="H2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
-        <v>243</v>
+      <c r="A3" s="46" t="s">
+        <v>272</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>9</v>
@@ -17586,19 +17857,19 @@
       <c r="C3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="H3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>38</v>
@@ -17607,40 +17878,40 @@
         <v>0</v>
       </c>
       <c r="D4" s="17"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="46" t="n">
+      <c r="E4" s="38"/>
+      <c r="F4" s="47" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47" t="s">
-        <v>246</v>
+      <c r="A5" s="48" t="s">
+        <v>275</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>247</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="E5" s="41"/>
+        <v>276</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5" s="36"/>
       <c r="F5" s="28" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="H5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
-        <v>252</v>
+      <c r="A6" s="37" t="s">
+        <v>281</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>10</v>
@@ -17649,10 +17920,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="49" t="s">
-        <v>254</v>
+        <v>282</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>283</v>
       </c>
       <c r="F6" s="17" t="n">
         <v>4</v>
@@ -17661,8 +17932,8 @@
       <c r="H6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
-        <v>255</v>
+      <c r="A7" s="39" t="s">
+        <v>284</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>38</v>
@@ -17671,10 +17942,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>6</v>
@@ -17683,8 +17954,8 @@
       <c r="H7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
-        <v>258</v>
+      <c r="A8" s="43" t="s">
+        <v>287</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>9</v>
@@ -17700,7 +17971,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -17710,7 +17981,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -17719,8 +17990,8 @@
       <c r="F10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
-        <v>261</v>
+      <c r="A11" s="39" t="s">
+        <v>290</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>10</v>
@@ -17729,10 +18000,10 @@
         <v>49</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>2</v>
@@ -17740,8 +18011,8 @@
       <c r="H11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
-        <v>264</v>
+      <c r="A12" s="39" t="s">
+        <v>293</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>43</v>
@@ -17750,13 +18021,13 @@
         <v>49</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>267</v>
+        <v>296</v>
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
@@ -18688,9 +18959,9 @@
       <selection pane="bottomLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="50" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="51" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.14"/>
@@ -18700,7 +18971,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>268</v>
+        <v>297</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -18725,8 +18996,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="s">
-        <v>269</v>
+      <c r="A2" s="52" t="s">
+        <v>298</v>
       </c>
       <c r="B2" s="14" t="n">
         <v>0</v>
@@ -18735,18 +19006,18 @@
         <v>0</v>
       </c>
       <c r="D2" s="17"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="52" t="n">
+      <c r="E2" s="44"/>
+      <c r="F2" s="53" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>270</v>
+        <v>299</v>
       </c>
       <c r="H2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
-        <v>271</v>
+      <c r="A3" s="52" t="s">
+        <v>300</v>
       </c>
       <c r="B3" s="14" t="n">
         <v>0</v>
@@ -18755,22 +19026,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="52" t="n">
+        <v>301</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="53" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>273</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
-        <v>274</v>
+      <c r="A4" s="52" t="s">
+        <v>303</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -18779,20 +19050,20 @@
         <v>0</v>
       </c>
       <c r="D4" s="17"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="52" t="n">
+      <c r="E4" s="44"/>
+      <c r="F4" s="53" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>275</v>
+        <v>304</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>276</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
-        <v>277</v>
+      <c r="A5" s="52" t="s">
+        <v>306</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>38</v>
@@ -18801,20 +19072,20 @@
         <v>0</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="52" t="n">
+      <c r="E5" s="44"/>
+      <c r="F5" s="53" t="n">
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>278</v>
+        <v>307</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="s">
-        <v>280</v>
+      <c r="A6" s="52" t="s">
+        <v>309</v>
       </c>
       <c r="B6" s="14" t="n">
         <v>0</v>
@@ -18822,23 +19093,23 @@
       <c r="C6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>281</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="52" t="n">
+      <c r="D6" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="53" t="n">
         <v>3</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>56</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>282</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="50" t="s">
-        <v>283</v>
+      <c r="A7" s="51" t="s">
+        <v>312</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>9</v>
@@ -18847,22 +19118,22 @@
         <v>9</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="52" t="n">
+        <v>313</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="F7" s="53" t="n">
         <v>2</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>285</v>
+        <v>314</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>286</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="s">
-        <v>287</v>
+      <c r="A8" s="52" t="s">
+        <v>316</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>10</v>
@@ -18870,23 +19141,23 @@
       <c r="C8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="40" t="s">
-        <v>288</v>
-      </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="52" t="n">
+      <c r="D8" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="F8" s="53" t="n">
         <v>3</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>275</v>
+        <v>304</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>289</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="s">
-        <v>290</v>
+      <c r="A9" s="52" t="s">
+        <v>319</v>
       </c>
       <c r="B9" s="14" t="n">
         <v>0</v>
@@ -18894,8 +19165,8 @@
       <c r="C9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>291</v>
+      <c r="D9" s="38" t="s">
+        <v>320</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="11" t="n">
@@ -18905,15 +19176,15 @@
         <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="s">
-        <v>293</v>
+      <c r="A10" s="52" t="s">
+        <v>322</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>38</v>
@@ -18921,65 +19192,65 @@
       <c r="C10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="40" t="s">
-        <v>294</v>
-      </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="52" t="n">
+      <c r="D10" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="E10" s="44"/>
+      <c r="F10" s="53" t="n">
         <v>3</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>296</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
-        <v>297</v>
+      <c r="A11" s="48" t="s">
+        <v>326</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>298</v>
-      </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54" t="n">
+        <v>59</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55" t="n">
         <v>4</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>299</v>
+        <v>328</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>300</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>301</v>
+      <c r="A12" s="37" t="s">
+        <v>330</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="52" t="n">
+        <v>59</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="E12" s="44"/>
+      <c r="F12" s="53" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>303</v>
+      <c r="A13" s="37" t="s">
+        <v>332</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>49</v>
@@ -18987,20 +19258,20 @@
       <c r="C13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="52" t="n">
+      <c r="D13" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="E13" s="44"/>
+      <c r="F13" s="53" t="n">
         <v>6</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
-        <v>306</v>
+      <c r="A14" s="37" t="s">
+        <v>335</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>10</v>
@@ -19008,17 +19279,17 @@
       <c r="C14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="52" t="n">
+      <c r="D14" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="E14" s="44"/>
+      <c r="F14" s="53" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="s">
-        <v>308</v>
+      <c r="A15" s="37" t="s">
+        <v>337</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>49</v>
@@ -19026,20 +19297,20 @@
       <c r="C15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="40" t="s">
-        <v>309</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="52" t="n">
+      <c r="D15" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="E15" s="44"/>
+      <c r="F15" s="53" t="n">
         <v>8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="s">
-        <v>311</v>
+      <c r="A16" s="37" t="s">
+        <v>340</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>38</v>
@@ -19047,33 +19318,33 @@
       <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="40" t="s">
-        <v>312</v>
+      <c r="D16" s="38" t="s">
+        <v>341</v>
       </c>
       <c r="E16" s="18"/>
-      <c r="F16" s="51" t="n">
+      <c r="F16" s="52" t="n">
         <v>8</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
-      <c r="K16" s="40"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
       <c r="E17" s="18"/>
-      <c r="F17" s="51" t="n">
+      <c r="F17" s="52" t="n">
         <v>7</v>
       </c>
       <c r="G17" s="0"/>
@@ -19083,29 +19354,29 @@
       <c r="K17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
-        <v>315</v>
+      <c r="A18" s="39" t="s">
+        <v>344</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="E18" s="18"/>
-      <c r="F18" s="51" t="n">
+      <c r="F18" s="52" t="n">
         <v>6</v>
       </c>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
-      <c r="K18" s="40"/>
+      <c r="K18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>38</v>
@@ -19114,21 +19385,21 @@
         <v>43</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>318</v>
+        <v>347</v>
       </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="51" t="n">
+      <c r="F19" s="52" t="n">
         <v>8</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="15"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
-      <c r="K19" s="40"/>
+      <c r="K19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
-        <v>319</v>
+      <c r="A20" s="39" t="s">
+        <v>348</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>10</v>
@@ -19137,18 +19408,18 @@
         <v>0</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>320</v>
+        <v>349</v>
       </c>
       <c r="E20" s="18"/>
-      <c r="F20" s="51" t="n">
+      <c r="F20" s="52" t="n">
         <v>4</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="37" t="s">
-        <v>321</v>
+      <c r="A21" s="39" t="s">
+        <v>350</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>38</v>
@@ -19157,16 +19428,16 @@
         <v>10</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="55" t="n">
+      <c r="F21" s="42" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
-        <v>323</v>
+      <c r="A22" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="B22" s="14" t="n">
         <v>0</v>
@@ -19175,18 +19446,18 @@
         <v>38</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="F22" s="55" t="s">
-        <v>326</v>
+        <v>354</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>10</v>
@@ -19194,19 +19465,19 @@
       <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="45" t="s">
-        <v>328</v>
-      </c>
-      <c r="E23" s="45" t="s">
-        <v>329</v>
-      </c>
-      <c r="F23" s="50" t="n">
+      <c r="D23" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="F23" s="51" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37" t="s">
-        <v>330</v>
+      <c r="A24" s="39" t="s">
+        <v>359</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>38</v>
@@ -19215,15 +19486,15 @@
         <v>19</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="F24" s="50" t="n">
+        <v>360</v>
+      </c>
+      <c r="F24" s="51" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
-        <v>332</v>
+      <c r="A25" s="39" t="s">
+        <v>361</v>
       </c>
       <c r="B25" s="14" t="n">
         <v>0</v>
@@ -19232,16 +19503,16 @@
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>333</v>
+        <v>362</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="50" t="n">
+      <c r="F25" s="51" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37" t="s">
-        <v>334</v>
+      <c r="A26" s="39" t="s">
+        <v>363</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>49</v>
@@ -19250,26 +19521,26 @@
         <v>19</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="F26" s="50" t="n">
+        <v>364</v>
+      </c>
+      <c r="F26" s="51" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>336</v>
+      <c r="A27" s="39" t="s">
+        <v>365</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>337</v>
-      </c>
-      <c r="F27" s="50" t="n">
+        <v>366</v>
+      </c>
+      <c r="F27" s="51" t="n">
         <v>8</v>
       </c>
     </row>
@@ -20272,16 +20543,16 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="50" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="51" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="50" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="50" width="29.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="50" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="51" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="29.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="51" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="54.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="3" width="8.54"/>
@@ -20289,7 +20560,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>338</v>
+        <v>367</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -20307,7 +20578,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>339</v>
+        <v>368</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>7</v>
@@ -21330,8 +21601,8 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
-        <v>340</v>
+      <c r="A2" s="51" t="s">
+        <v>369</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0</v>
@@ -21340,14 +21611,14 @@
         <v>0</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="50" t="n">
+      <c r="E2" s="46"/>
+      <c r="F2" s="51" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="H2" s="42"/>
+        <v>304</v>
+      </c>
+      <c r="H2" s="44"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -22366,8 +22637,8 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="50" t="s">
-        <v>341</v>
+      <c r="A3" s="51" t="s">
+        <v>370</v>
       </c>
       <c r="B3" s="14" t="n">
         <v>0</v>
@@ -22376,14 +22647,14 @@
         <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="50" t="n">
+        <v>371</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="51" t="n">
         <v>3</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>343</v>
+        <v>372</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
@@ -23404,28 +23675,28 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
-        <v>344</v>
+      <c r="A4" s="52" t="s">
+        <v>373</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51" t="n">
+        <v>374</v>
+      </c>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
-      <c r="J4" s="44"/>
+      <c r="J4" s="46"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="5"/>
@@ -24442,8 +24713,8 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="50" t="s">
-        <v>346</v>
+      <c r="A5" s="51" t="s">
+        <v>375</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>38</v>
@@ -24452,13 +24723,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="F5" s="50" t="n">
+        <v>376</v>
+      </c>
+      <c r="F5" s="51" t="n">
         <v>3</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>348</v>
+        <v>377</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
@@ -25479,8 +25750,8 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="s">
-        <v>349</v>
+      <c r="A6" s="52" t="s">
+        <v>378</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>38</v>
@@ -25489,13 +25760,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="F6" s="50" t="n">
+        <v>379</v>
+      </c>
+      <c r="F6" s="51" t="n">
         <v>3</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>351</v>
+        <v>380</v>
       </c>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
@@ -26516,8 +26787,8 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="s">
-        <v>352</v>
+      <c r="A7" s="52" t="s">
+        <v>381</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>10</v>
@@ -26526,14 +26797,14 @@
         <v>38</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51" t="n">
+        <v>382</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52" t="n">
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>285</v>
+        <v>314</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
@@ -27554,8 +27825,8 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="s">
-        <v>354</v>
+      <c r="A8" s="52" t="s">
+        <v>383</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>10</v>
@@ -27564,14 +27835,14 @@
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51" t="n">
+        <v>384</v>
+      </c>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52" t="n">
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
@@ -28592,8 +28863,8 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="s">
-        <v>357</v>
+      <c r="A9" s="52" t="s">
+        <v>386</v>
       </c>
       <c r="B9" s="14" t="n">
         <v>0</v>
@@ -28602,14 +28873,14 @@
         <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51" t="n">
+        <v>387</v>
+      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52" t="n">
         <v>4</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
@@ -29630,8 +29901,8 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="s">
-        <v>360</v>
+      <c r="A10" s="52" t="s">
+        <v>389</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>9</v>
@@ -29640,14 +29911,14 @@
         <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51" t="n">
+        <v>390</v>
+      </c>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52" t="n">
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
@@ -30668,8 +30939,8 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51" t="s">
-        <v>362</v>
+      <c r="A11" s="52" t="s">
+        <v>391</v>
       </c>
       <c r="B11" s="14" t="n">
         <v>0</v>
@@ -30678,14 +30949,14 @@
         <v>0</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51" t="n">
+        <v>392</v>
+      </c>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52" t="n">
         <v>4</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
@@ -31706,8 +31977,8 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44" t="s">
-        <v>365</v>
+      <c r="A12" s="46" t="s">
+        <v>394</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>49</v>
@@ -31716,9 +31987,9 @@
         <v>49</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="F12" s="50" t="n">
+        <v>395</v>
+      </c>
+      <c r="F12" s="51" t="n">
         <v>5</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -32743,8 +33014,8 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="51" t="s">
-        <v>367</v>
+      <c r="A13" s="52" t="s">
+        <v>396</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>43</v>
@@ -32753,14 +33024,14 @@
         <v>9</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>368</v>
-      </c>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51" t="n">
+        <v>397</v>
+      </c>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>369</v>
+        <v>398</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
@@ -33781,8 +34052,8 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50" t="s">
-        <v>370</v>
+      <c r="A14" s="51" t="s">
+        <v>399</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>9</v>
@@ -33791,21 +34062,21 @@
         <v>10</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="F14" s="50" t="n">
+        <v>400</v>
+      </c>
+      <c r="F14" s="51" t="n">
         <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>372</v>
+        <v>401</v>
       </c>
       <c r="H14" s="0"/>
-      <c r="I14" s="50"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="19"/>
       <c r="K14" s="2"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
       <c r="O14" s="0"/>
       <c r="P14" s="0"/>
       <c r="Q14" s="0"/>
@@ -34818,8 +35089,8 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="50" t="s">
-        <v>373</v>
+      <c r="A15" s="51" t="s">
+        <v>402</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>9</v>
@@ -34828,21 +35099,21 @@
         <v>10</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="F15" s="50" t="n">
+        <v>403</v>
+      </c>
+      <c r="F15" s="51" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>348</v>
+        <v>377</v>
       </c>
       <c r="H15" s="0"/>
-      <c r="I15" s="50"/>
+      <c r="I15" s="51"/>
       <c r="J15" s="19"/>
       <c r="K15" s="2"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
       <c r="O15" s="0"/>
       <c r="P15" s="0"/>
       <c r="Q15" s="0"/>
@@ -35855,31 +36126,31 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="s">
-        <v>375</v>
+      <c r="A16" s="51" t="s">
+        <v>404</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="F16" s="50" t="n">
+        <v>374</v>
+      </c>
+      <c r="F16" s="51" t="n">
         <v>4</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>376</v>
+        <v>405</v>
       </c>
       <c r="H16" s="0"/>
-      <c r="I16" s="50"/>
+      <c r="I16" s="51"/>
       <c r="J16" s="19"/>
       <c r="K16" s="2"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
       <c r="O16" s="0"/>
       <c r="P16" s="0"/>
       <c r="Q16" s="0"/>
@@ -36892,8 +37163,8 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="50" t="s">
-        <v>377</v>
+      <c r="A17" s="51" t="s">
+        <v>406</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>9</v>
@@ -36902,21 +37173,21 @@
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="F17" s="50" t="n">
+        <v>407</v>
+      </c>
+      <c r="F17" s="51" t="n">
         <v>4</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="H17" s="0"/>
-      <c r="I17" s="50"/>
+      <c r="I17" s="51"/>
       <c r="J17" s="19"/>
       <c r="K17" s="2"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
       <c r="O17" s="0"/>
       <c r="P17" s="0"/>
       <c r="Q17" s="0"/>
@@ -37929,8 +38200,8 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="47" t="s">
-        <v>379</v>
+      <c r="A18" s="48" t="s">
+        <v>408</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>9</v>
@@ -37939,26 +38210,26 @@
         <v>10</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47" t="n">
+        <v>409</v>
+      </c>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48" t="n">
         <v>4</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="H18" s="27"/>
-      <c r="I18" s="50"/>
+      <c r="I18" s="51"/>
       <c r="J18" s="19"/>
       <c r="K18" s="2"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>381</v>
+      <c r="A19" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>10</v>
@@ -37967,25 +38238,25 @@
         <v>10</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51" t="n">
+        <v>411</v>
+      </c>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52" t="n">
         <v>7</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="I19" s="50"/>
+        <v>412</v>
+      </c>
+      <c r="I19" s="51"/>
       <c r="J19" s="19"/>
       <c r="K19" s="2"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
     </row>
     <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
-        <v>384</v>
+      <c r="A20" s="39" t="s">
+        <v>413</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>10</v>
@@ -37994,18 +38265,18 @@
         <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="F20" s="50" t="n">
+        <v>414</v>
+      </c>
+      <c r="F20" s="51" t="n">
         <v>7</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>386</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="37" t="s">
-        <v>387</v>
+      <c r="A21" s="39" t="s">
+        <v>416</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>10</v>
@@ -38014,13 +38285,13 @@
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="F21" s="50" t="n">
+        <v>417</v>
+      </c>
+      <c r="F21" s="51" t="n">
         <v>7</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>383</v>
+        <v>412</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
@@ -39041,8 +39312,8 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
-        <v>389</v>
+      <c r="A22" s="39" t="s">
+        <v>418</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>10</v>
@@ -39051,13 +39322,13 @@
         <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="F22" s="50" t="n">
+        <v>419</v>
+      </c>
+      <c r="F22" s="51" t="n">
         <v>7</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>383</v>
+        <v>412</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
@@ -40078,8 +40349,8 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="s">
-        <v>391</v>
+      <c r="A23" s="39" t="s">
+        <v>420</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>38</v>
@@ -40088,13 +40359,13 @@
         <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="F23" s="50" t="n">
+        <v>421</v>
+      </c>
+      <c r="F23" s="51" t="n">
         <v>8</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>393</v>
+        <v>422</v>
       </c>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
@@ -41115,8 +41386,8 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37" t="s">
-        <v>394</v>
+      <c r="A24" s="39" t="s">
+        <v>423</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>9</v>
@@ -41125,13 +41396,13 @@
         <v>10</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="F24" s="50" t="n">
+        <v>424</v>
+      </c>
+      <c r="F24" s="51" t="n">
         <v>7</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>396</v>
+        <v>425</v>
       </c>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
@@ -42152,8 +42423,8 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
-        <v>397</v>
+      <c r="A25" s="39" t="s">
+        <v>426</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>10</v>
@@ -42162,13 +42433,13 @@
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="F25" s="50" t="n">
+        <v>427</v>
+      </c>
+      <c r="F25" s="51" t="n">
         <v>7</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>399</v>
+        <v>428</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
@@ -43189,8 +43460,8 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36" t="s">
-        <v>400</v>
+      <c r="A26" s="37" t="s">
+        <v>429</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>43</v>
@@ -43199,14 +43470,14 @@
         <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51" t="n">
+        <v>430</v>
+      </c>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52" t="n">
         <v>5</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>402</v>
+        <v>431</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
@@ -44227,8 +44498,8 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>403</v>
+      <c r="A27" s="39" t="s">
+        <v>432</v>
       </c>
       <c r="B27" s="14" t="n">
         <v>0</v>
@@ -44237,13 +44508,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="F27" s="50" t="n">
+        <v>433</v>
+      </c>
+      <c r="F27" s="51" t="n">
         <v>8</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>405</v>
+        <v>434</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
@@ -45265,7 +45536,7 @@
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="56" t="s">
-        <v>406</v>
+        <v>435</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>10</v>
@@ -45274,18 +45545,18 @@
         <v>38</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="F28" s="50" t="n">
+        <v>436</v>
+      </c>
+      <c r="F28" s="51" t="n">
         <v>8</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>399</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
-        <v>408</v>
+      <c r="A29" s="39" t="s">
+        <v>437</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>9</v>
@@ -45294,18 +45565,18 @@
         <v>10</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>409</v>
-      </c>
-      <c r="F29" s="50" t="n">
+        <v>438</v>
+      </c>
+      <c r="F29" s="51" t="n">
         <v>5</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>299</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
-        <v>410</v>
+      <c r="A30" s="39" t="s">
+        <v>439</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>9</v>
@@ -45314,18 +45585,18 @@
         <v>10</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="F30" s="50" t="n">
+        <v>440</v>
+      </c>
+      <c r="F30" s="51" t="n">
         <v>5</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>299</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="37" t="s">
-        <v>412</v>
+      <c r="A31" s="39" t="s">
+        <v>441</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>49</v>
@@ -45334,18 +45605,18 @@
         <v>44</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="F31" s="50" t="n">
+        <v>442</v>
+      </c>
+      <c r="F31" s="51" t="n">
         <v>8</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>278</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="37" t="s">
-        <v>414</v>
+      <c r="A32" s="39" t="s">
+        <v>443</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>10</v>
@@ -45354,18 +45625,18 @@
         <v>38</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>415</v>
-      </c>
-      <c r="F32" s="50" t="n">
+        <v>444</v>
+      </c>
+      <c r="F32" s="51" t="n">
         <v>6</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>416</v>
+        <v>445</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="37" t="s">
-        <v>417</v>
+      <c r="A33" s="39" t="s">
+        <v>446</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>9</v>
@@ -45374,30 +45645,30 @@
         <v>49</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="F33" s="50" t="n">
+        <v>447</v>
+      </c>
+      <c r="F33" s="51" t="n">
         <v>7</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>419</v>
+        <v>448</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36" t="s">
-        <v>420</v>
+      <c r="A34" s="37" t="s">
+        <v>449</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>421</v>
-      </c>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51" t="n">
+        <v>450</v>
+      </c>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52" t="n">
         <v>10</v>
       </c>
       <c r="G34" s="57" t="s">
@@ -45407,7 +45678,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
@@ -45419,7 +45690,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
@@ -45431,7 +45702,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="31" t="s">
-        <v>422</v>
+        <v>451</v>
       </c>
       <c r="B37" s="31"/>
       <c r="C37" s="31"/>
@@ -45443,7 +45714,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31" t="s">
-        <v>423</v>
+        <v>452</v>
       </c>
       <c r="B38" s="31"/>
       <c r="C38" s="31"/>
@@ -45455,7 +45726,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="31" t="s">
-        <v>424</v>
+        <v>453</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -45465,9 +45736,9 @@
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
     </row>
-    <row r="40" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="37" t="s">
-        <v>425</v>
+    <row r="40" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="39" t="s">
+        <v>454</v>
       </c>
       <c r="B40" s="14" t="n">
         <v>0</v>
@@ -45476,12 +45747,12 @@
         <v>84</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="E40" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="F40" s="50" t="n">
+        <v>455</v>
+      </c>
+      <c r="E40" s="51" t="s">
+        <v>456</v>
+      </c>
+      <c r="F40" s="51" t="n">
         <v>10</v>
       </c>
       <c r="G40" s="57" t="s">
@@ -46215,13 +46486,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.58"/>
@@ -46233,7 +46504,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>428</v>
+        <v>457</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -46259,7 +46530,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>429</v>
+        <v>458</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0</v>
@@ -46268,20 +46539,20 @@
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>430</v>
+        <v>459</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>431</v>
+        <v>460</v>
       </c>
       <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>432</v>
+        <v>461</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>9</v>
@@ -46290,20 +46561,20 @@
         <v>9</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>433</v>
+        <v>462</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="4" t="n">
         <v>3</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>270</v>
+        <v>299</v>
       </c>
       <c r="H3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>434</v>
+        <v>463</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>9</v>
@@ -46312,7 +46583,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>430</v>
+        <v>459</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="4" t="n">
@@ -46325,7 +46596,7 @@
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>435</v>
+        <v>464</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>38</v>
@@ -46334,7 +46605,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>436</v>
+        <v>465</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="4" t="n">
@@ -46345,7 +46616,7 @@
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>437</v>
+        <v>466</v>
       </c>
       <c r="B6" s="14" t="n">
         <v>0</v>
@@ -46354,7 +46625,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>438</v>
+        <v>467</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="4" t="n">
@@ -46365,7 +46636,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>439</v>
+        <v>468</v>
       </c>
       <c r="B7" s="14" t="n">
         <v>0</v>
@@ -46374,20 +46645,20 @@
         <v>0</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="H7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>442</v>
+        <v>471</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>38</v>
@@ -46396,7 +46667,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="4" t="n">
@@ -46409,7 +46680,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="58" t="s">
-        <v>443</v>
+        <v>472</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>19</v>
@@ -46418,20 +46689,20 @@
         <v>0</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>444</v>
+        <v>473</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="46" t="s">
-        <v>224</v>
+      <c r="G9" s="47" t="s">
+        <v>253</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="58" t="s">
-        <v>445</v>
+        <v>474</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>38</v>
@@ -46440,20 +46711,20 @@
         <v>0</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>446</v>
+        <v>475</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G10" s="46" t="s">
-        <v>285</v>
+      <c r="G10" s="47" t="s">
+        <v>314</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="58" t="s">
-        <v>447</v>
+        <v>476</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>10</v>
@@ -46462,20 +46733,20 @@
         <v>0</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>448</v>
+        <v>477</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G11" s="46" t="s">
-        <v>224</v>
+      <c r="G11" s="47" t="s">
+        <v>253</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="58" t="s">
-        <v>449</v>
+        <v>478</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>38</v>
@@ -46484,16 +46755,24 @@
         <v>0</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>450</v>
+        <v>479</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G12" s="46" t="s">
-        <v>285</v>
+      <c r="G12" s="47" t="s">
+        <v>314</v>
       </c>
       <c r="H12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>481</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10">

</xml_diff>